<commit_message>
added some error handling and added functionality to save errors into error.log
</commit_message>
<xml_diff>
--- a/Playbook_Template.xlsx
+++ b/Playbook_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>device_type</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>Config_Commands</t>
-  </si>
-  <si>
-    <t>david</t>
   </si>
   <si>
     <t>show start
@@ -266,7 +263,7 @@
 show interfaces status</t>
   </si>
   <si>
-    <t>X.X.X.X</t>
+    <t>x.x.x.x</t>
   </si>
 </sst>
 </file>
@@ -623,7 +620,7 @@
   <dimension ref="A1:CH3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,13 +939,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="O2" s="2"/>
     </row>
@@ -957,13 +951,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="1"/>
     </row>

</xml_diff>